<commit_message>
batru P3,P4 templates update
</commit_message>
<xml_diff>
--- a/Projects/BATRU/Data/P3_template.xlsx
+++ b/Projects/BATRU/Data/P3_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,16 +18,16 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$511</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
@@ -37,6 +37,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
@@ -51,6 +52,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
@@ -65,11 +67,12 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
@@ -79,6 +82,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
@@ -93,6 +97,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
@@ -107,6 +112,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -118,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4572" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="364">
   <si>
     <t>State</t>
   </si>
@@ -1152,64 +1158,64 @@
     <t>ALL</t>
   </si>
   <si>
-    <t>GC_A_TN_Shelf Strip for SAS - Kent_DL3</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Shelf Strip for SAS - Kent_DL3 (1), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (10), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (11), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (12), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (13), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (14), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (15), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (16), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (17), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (18), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (19), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (2), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (20), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (21), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (22), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (23), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (24), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (25), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (26), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (3), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (4), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (5), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (6), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (7), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (8), GC_A_TN_Shelf Strip for SAS - Kent_DL3 (9)</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD - Kent_DL_new</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD - Kent_DL_new (1)</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Shelf Strip for SAS - Kent_DL_new</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Shelf Strip for SAS - Kent_DL_new (1), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (10), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (11), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (12), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (13), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (14), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (15), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (16), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (17), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (18), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (19), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (2), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (20), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (21), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (22), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (23), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (24), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (25), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (26), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (3), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (4), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (5), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (6), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (7), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (8), GC_A_TN_Shelf Strip for SAS - Kent_DL_new (9)</t>
-  </si>
-  <si>
-    <t>GC_A_TN_BackGround_for_BWD - Rtm_Mandarin</t>
-  </si>
-  <si>
-    <t>B_RTH_Stickers_BWD_Asymmetric_305x155, B_RTH_Stickers_BWD_Asymmetric_356x155, B_RTH_Stickers_BWD_Asymmetric_485x155, B_RTH_Stickers_BWD_Asymmetric_500x155, B_RTH_Stickers_BWD_Asymmetric_680x155, B_RTH_Stickers_BWD_Symmetric_238x155-03, B_RTH_Stickers_BWD_Symmetric_238x155-04, B_RTH_Stickers_BWD_Symmetric_268x100-05, B_RTH_Stickers_BWD_Symmetric_268x100-06, B_RTH_Stickers_BWD_Symmetric_321x155-01, B_RTH_Stickers_BWD_Symmetric_321x155-02</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD - Rtm_Mandarin</t>
-  </si>
-  <si>
-    <t>BAT_RTH_SAS_Vert_306x274-2, BAT_RTH_SAS_Vert_306x274</t>
-  </si>
-  <si>
-    <t>GC_A_TN_PHL - Rtm_Mandarin</t>
-  </si>
-  <si>
-    <t>B_RTH_Moсkup_152x160-1, B_RTH_Moсkup_152x160-2, B_RTH_Moсkup_3008_152x160-1, B_RTH_Moсkup_3008_152x160-2</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Shelf Strip for SAS - Rtm_Mandarin</t>
-  </si>
-  <si>
-    <t>B_RTH_Stripe_Cupsule_3008_178x48, B_RTH_Stripe_Cupsule_3008_238x48, B_RTH_Stripe_Cupsule_3008_268x48, B_RTH_Stripe_Cupsule_3008_305x48, B_RTH_Stripe_Cupsule_3008_321x48, B_RTH_Stripe_Cupsule_3008_365x48, B_RTH_Stripe_Cupsule_3008_485x48, B_RTH_Stripe_Cupsule_3008_500x48, B_RTH_Stripe_Cupsule_3008_680x48, B_RTH_Stripe_Letters_178x25, B_RTH_Stripe_Letters_238x25, B_RTH_Stripe_Letters_268x25, B_RTH_Stripe_Letters_305x25, B_RTH_Stripe_Letters_321x25, B_RTH_Stripe_Letters_365x25, B_RTH_Stripe_Letters_485x25, B_RTH_Stripe_Letters_500x25, B_RTH_Stripe_Letters_680x25</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD gor. - Kent_DL3</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD gor - Kent_DL3</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD gor. - Kent_DL_new</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD gor - Kent_DL_new (1)</t>
-  </si>
-  <si>
-    <t>GC_A_TN_Carboard SAS for BWD gor. - Rtm_Mandarin</t>
-  </si>
-  <si>
-    <t>BAT_RTH_SAS_Hor_278x190-2, BAT_RTH_SAS_Hor_278x190</t>
+    <t>GC_A_TN_SAS Frame - Kent_Amber</t>
+  </si>
+  <si>
+    <t>GC_A_TN_SAS Frame - Kent_Amber (1).jpg, GC_A_TN_SAS Frame - Kent_Amber (10).jpg, GC_A_TN_SAS Frame - Kent_Amber (2).jpg, GC_A_TN_SAS Frame - Kent_Amber (3).jpg, GC_A_TN_SAS Frame - Kent_Amber (4).jpg, GC_A_TN_SAS Frame - Kent_Amber (5).jpg, GC_A_TN_SAS Frame - Kent_Amber (6).jpg, GC_A_TN_SAS Frame - Kent_Amber (7).jpg, GC_A_TN_SAS Frame - Kent_Amber (8).jpg, GC_A_TN_SAS Frame - Kent_Amber (9).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Shelf Strip for SAS - Kent_Amber</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Shelf Strip for SAS - Kent_Amber.jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_SAS Frame - RTM_International</t>
+  </si>
+  <si>
+    <t>GC_A_TN_SAS Frame - RTM_International (1).jpg, GC_A_TN_SAS Frame - RTM_International (2).jpg, GC_A_TN_SAS Frame - RTM_International (3).jpg, GC_A_TN_SAS Frame - RTM_International (4).jpg, GC_A_TN_SAS Frame - RTM_International (5).jpg, GC_A_TN_SAS Frame - RTM_International (6).jpg, GC_A_TN_SAS Frame - RTM_International (7).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_BackGround_for_BWD - Kent_Amber</t>
+  </si>
+  <si>
+    <t>GC_A_TN_BackGround_for_BWD - Kent_Amber (1).jpg, GC_A_TN_BackGround_for_BWD - Kent_Amber (2).jpg, GC_A_TN_BackGround_for_BWD - Kent_Amber (3).jpg, GC_A_TN_BackGround_for_BWD - Kent_Amber (4).jpg, GC_A_TN_BackGround_for_BWD - Kent_Amber (5).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD - Kent_Amber</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD - Kent_Amber (1).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_BackGround_for_BWD - RTM_International</t>
+  </si>
+  <si>
+    <t>GC_A_TN_BackGround_for_BWD - RTM_International (1).jpg, GC_A_TN_BackGround_for_BWD - RTM_International (2).jpg, GC_A_TN_BackGround_for_BWD - RTM_International (3).jpg, GC_A_TN_BackGround_for_BWD - RTM_International (4).jpg, GC_A_TN_BackGround_for_BWD - RTM_International (5).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD - RTM_International</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD - RTM_International (1).jpg, GC_A_TN_Carboard SAS for BWD - RTM_International (2).jpg, GC_A_TN_Carboard SAS for BWD - RTM_International (3).jpg, GC_A_TN_Carboard SAS for BWD - RTM_International (4).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Shelf Strip for SAS - RTM_International</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Shelf Strip for SAS - RTM_International (1).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (2).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (3).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (4).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (5).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (6).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (7).jpg, GC_A_TN_Shelf Strip for SAS - RTM_International (8).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD gor. - Kent_Amber</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD gor. - Kent_Amber (1).jpg, GC_A_TN_Carboard SAS for BWD gor. - Kent_Amber (2).jpg</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD gor. - RTM_International</t>
+  </si>
+  <si>
+    <t>GC_A_TN_Carboard SAS for BWD gor. - RTM_International.jpg</t>
   </si>
 </sst>
 </file>
@@ -1695,15 +1701,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>473400</xdr:colOff>
+      <xdr:colOff>500400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>735120</xdr:colOff>
+      <xdr:colOff>761760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1716,8 +1722,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30029400" y="1440"/>
-          <a:ext cx="2547720" cy="172080"/>
+          <a:off x="30208680" y="1440"/>
+          <a:ext cx="2547360" cy="171720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1732,15 +1738,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>722520</xdr:colOff>
+      <xdr:colOff>749520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>724680</xdr:colOff>
+      <xdr:colOff>751320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1753,8 +1759,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29516400" y="36000"/>
-          <a:ext cx="4574160" cy="101520"/>
+          <a:off x="29695680" y="27000"/>
+          <a:ext cx="4573800" cy="101160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1769,15 +1775,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>492480</xdr:colOff>
+      <xdr:colOff>519480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>677880</xdr:colOff>
+      <xdr:colOff>704520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1790,8 +1796,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="32334480" y="3240"/>
-          <a:ext cx="2471400" cy="170280"/>
+          <a:off x="32513760" y="3240"/>
+          <a:ext cx="2471040" cy="169920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1839,19 +1845,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3846153846154"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
@@ -24783,7 +24789,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N521"/>
+  <autoFilter ref="A1:N511"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -24808,10 +24814,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.69635627530364"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8987854251012"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27355,10 +27361,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.8582995951417"/>
     <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.64372469635628"/>
@@ -28244,10 +28250,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -29622,7 +29628,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D43"/>
+  <autoFilter ref="A1:D41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -29647,8 +29653,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="44.1336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3157894736842"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.64372469635628"/>
@@ -30364,9 +30370,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.5222672064777"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.0566801619433"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -31003,19 +31009,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.0931174089069"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="93.2995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5222672064777"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="94.1578947368421"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -31038,13 +31044,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>344</v>
@@ -31055,7 +31061,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>69</v>
@@ -31072,13 +31078,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>348</v>
@@ -31089,13 +31095,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>350</v>
@@ -31106,13 +31112,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>352</v>
@@ -31123,10 +31129,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>46</v>
@@ -31140,10 +31146,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>46</v>
@@ -31157,302 +31163,302 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>343</v>
+        <v>46</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>117</v>
+        <v>15</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>343</v>
+        <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>350</v>
@@ -31463,27 +31469,27 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>46</v>
@@ -31497,903 +31503,308 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>343</v>
+        <v>46</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>343</v>
+        <v>16</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>343</v>
+        <v>46</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>343</v>
+        <v>46</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="E66" s="0" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="E75" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="E81" s="0" t="s">
-        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix state and attr3 in batru
</commit_message>
<xml_diff>
--- a/Projects/BATRU/Data/P3_template.xlsx
+++ b/Projects/BATRU/Data/P3_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,18 +18,18 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$511</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$521</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$511</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
@@ -55,6 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$A$1:$E$149</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
@@ -71,13 +73,14 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$68</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$43</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
@@ -87,6 +90,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$41</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
@@ -103,6 +107,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$61</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
@@ -119,6 +124,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -130,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="392">
   <si>
     <t>State</t>
   </si>
@@ -174,7 +180,7 @@
     <t>end_sequence</t>
   </si>
   <si>
-    <t>All</t>
+    <t>ALL</t>
   </si>
   <si>
     <t>GC_P_BWD Premium black 11x12</t>
@@ -1246,9 +1252,6 @@
   </si>
   <si>
     <t>Names of template in SR</t>
-  </si>
-  <si>
-    <t>ALL</t>
   </si>
   <si>
     <t>GC_A_TN_SAS Frame - Kent_Amber</t>
@@ -1574,11 +1577,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1790,15 +1793,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>527400</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>761400</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1811,8 +1814,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30942000" y="1440"/>
-          <a:ext cx="2604240" cy="171360"/>
+          <a:off x="31178520" y="1440"/>
+          <a:ext cx="2603880" cy="171000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1827,15 +1830,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>749520</xdr:colOff>
+      <xdr:colOff>776520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>777600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1848,8 +1851,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30410280" y="27000"/>
-          <a:ext cx="4687560" cy="100800"/>
+          <a:off x="30646800" y="18000"/>
+          <a:ext cx="4687200" cy="100440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1864,15 +1867,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>519480</xdr:colOff>
+      <xdr:colOff>546480</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>704160</xdr:colOff>
+      <xdr:colOff>730800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1885,8 +1888,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33304320" y="3240"/>
-          <a:ext cx="2527920" cy="169560"/>
+          <a:off x="33540840" y="3240"/>
+          <a:ext cx="2527560" cy="169200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1928,27 +1931,27 @@
   </sheetPr>
   <dimension ref="A1:O521"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -7718,13 +7721,13 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B132" s="11" t="s">
+      <c r="A132" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B132" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C132" s="10" t="n">
+      <c r="C132" s="11" t="n">
         <v>9</v>
       </c>
       <c r="D132" s="12" t="s">
@@ -7742,22 +7745,22 @@
       <c r="H132" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I132" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J132" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K132" s="10" t="n">
+      <c r="I132" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J132" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K132" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="L132" s="10" t="n">
+      <c r="L132" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="M132" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="N132" s="10" t="n">
+      <c r="M132" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="N132" s="11" t="n">
         <v>11</v>
       </c>
     </row>
@@ -24878,7 +24881,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N521"/>
+  <autoFilter ref="A1:N511"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -24897,16 +24900,16 @@
   </sheetPr>
   <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A211" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A234" activeCellId="0" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -28486,10 +28489,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.8582995951417"/>
     <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.64372469635628"/>
@@ -28594,7 +28597,7 @@
       <c r="B8" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="11" t="n">
         <v>7</v>
       </c>
       <c r="D8" s="21"/>
@@ -28607,7 +28610,7 @@
       <c r="B9" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="11" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="21"/>
@@ -28620,7 +28623,7 @@
       <c r="B10" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="11" t="n">
         <v>9</v>
       </c>
       <c r="D10" s="21"/>
@@ -28633,7 +28636,7 @@
       <c r="B11" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="11" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="21"/>
@@ -28646,7 +28649,7 @@
       <c r="B12" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="11" t="n">
         <v>11</v>
       </c>
       <c r="D12" s="21"/>
@@ -28659,7 +28662,7 @@
       <c r="B13" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="11" t="n">
         <v>12</v>
       </c>
       <c r="D13" s="21"/>
@@ -28672,7 +28675,7 @@
       <c r="B14" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="11" t="n">
         <v>13</v>
       </c>
       <c r="D14" s="21"/>
@@ -28685,7 +28688,7 @@
       <c r="B15" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="11" t="n">
         <v>14</v>
       </c>
       <c r="D15" s="21"/>
@@ -28698,7 +28701,7 @@
       <c r="B16" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="11" t="n">
         <v>15</v>
       </c>
       <c r="D16" s="21"/>
@@ -28711,7 +28714,7 @@
       <c r="B17" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="11" t="n">
         <v>16</v>
       </c>
       <c r="D17" s="21"/>
@@ -28724,7 +28727,7 @@
       <c r="B18" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="11" t="n">
         <v>17</v>
       </c>
       <c r="D18" s="21"/>
@@ -28737,7 +28740,7 @@
       <c r="B19" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="11" t="n">
         <v>18</v>
       </c>
       <c r="D19" s="21"/>
@@ -28750,7 +28753,7 @@
       <c r="B20" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="11" t="n">
         <v>19</v>
       </c>
       <c r="D20" s="21"/>
@@ -28763,7 +28766,7 @@
       <c r="B21" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="11" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="30"/>
@@ -28776,7 +28779,7 @@
       <c r="B22" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="11" t="n">
         <v>21</v>
       </c>
       <c r="D22" s="30"/>
@@ -28789,7 +28792,7 @@
       <c r="B23" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="11" t="n">
         <v>22</v>
       </c>
       <c r="D23" s="30"/>
@@ -28802,7 +28805,7 @@
       <c r="B24" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="11" t="n">
         <v>23</v>
       </c>
       <c r="D24" s="30"/>
@@ -28815,7 +28818,7 @@
       <c r="B25" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="11" t="n">
         <v>24</v>
       </c>
       <c r="D25" s="30"/>
@@ -28828,7 +28831,7 @@
       <c r="B26" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="C26" s="10" t="n">
+      <c r="C26" s="11" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="30"/>
@@ -28841,7 +28844,7 @@
       <c r="B27" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="11" t="n">
         <v>26</v>
       </c>
       <c r="D27" s="30"/>
@@ -28854,7 +28857,7 @@
       <c r="B28" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="11" t="n">
         <v>27</v>
       </c>
       <c r="D28" s="30"/>
@@ -28867,7 +28870,7 @@
       <c r="B29" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="11" t="n">
         <v>28</v>
       </c>
       <c r="D29" s="30"/>
@@ -28880,7 +28883,7 @@
       <c r="B30" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="10" t="n">
+      <c r="C30" s="11" t="n">
         <v>29</v>
       </c>
       <c r="D30" s="30"/>
@@ -28893,7 +28896,7 @@
       <c r="B31" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="C31" s="10" t="n">
+      <c r="C31" s="11" t="n">
         <v>30</v>
       </c>
       <c r="D31" s="30"/>
@@ -28906,7 +28909,7 @@
       <c r="B32" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="C32" s="10" t="n">
+      <c r="C32" s="11" t="n">
         <v>31</v>
       </c>
       <c r="D32" s="30"/>
@@ -28919,7 +28922,7 @@
       <c r="B33" s="29" t="s">
         <v>279</v>
       </c>
-      <c r="C33" s="10" t="n">
+      <c r="C33" s="11" t="n">
         <v>32</v>
       </c>
       <c r="D33" s="30"/>
@@ -28932,7 +28935,7 @@
       <c r="B34" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="C34" s="10" t="n">
+      <c r="C34" s="11" t="n">
         <v>33</v>
       </c>
       <c r="D34" s="30"/>
@@ -28945,7 +28948,7 @@
       <c r="B35" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="C35" s="10" t="n">
+      <c r="C35" s="11" t="n">
         <v>34</v>
       </c>
       <c r="D35" s="30"/>
@@ -28958,7 +28961,7 @@
       <c r="B36" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="C36" s="10" t="n">
+      <c r="C36" s="11" t="n">
         <v>35</v>
       </c>
       <c r="D36" s="30"/>
@@ -28971,7 +28974,7 @@
       <c r="B37" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="C37" s="10" t="n">
+      <c r="C37" s="11" t="n">
         <v>36</v>
       </c>
       <c r="D37" s="30"/>
@@ -28984,7 +28987,7 @@
       <c r="B38" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="C38" s="10" t="n">
+      <c r="C38" s="11" t="n">
         <v>37</v>
       </c>
       <c r="D38" s="30"/>
@@ -28997,7 +29000,7 @@
       <c r="B39" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="10" t="n">
+      <c r="C39" s="11" t="n">
         <v>38</v>
       </c>
       <c r="D39" s="30"/>
@@ -29010,7 +29013,7 @@
       <c r="B40" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="C40" s="10" t="n">
+      <c r="C40" s="11" t="n">
         <v>39</v>
       </c>
       <c r="D40" s="30"/>
@@ -29023,7 +29026,7 @@
       <c r="B41" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C41" s="10" t="n">
+      <c r="C41" s="11" t="n">
         <v>40</v>
       </c>
       <c r="D41" s="30"/>
@@ -29036,7 +29039,7 @@
       <c r="B42" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="10" t="n">
+      <c r="C42" s="11" t="n">
         <v>41</v>
       </c>
       <c r="D42" s="30"/>
@@ -29049,7 +29052,7 @@
       <c r="B43" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="10" t="n">
+      <c r="C43" s="11" t="n">
         <v>42</v>
       </c>
       <c r="D43" s="30"/>
@@ -29062,7 +29065,7 @@
       <c r="B44" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="C44" s="10" t="n">
+      <c r="C44" s="11" t="n">
         <v>43</v>
       </c>
       <c r="D44" s="30"/>
@@ -29075,7 +29078,7 @@
       <c r="B45" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="C45" s="10" t="n">
+      <c r="C45" s="11" t="n">
         <v>44</v>
       </c>
       <c r="D45" s="30"/>
@@ -29088,7 +29091,7 @@
       <c r="B46" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="C46" s="10" t="n">
+      <c r="C46" s="11" t="n">
         <v>45</v>
       </c>
       <c r="D46" s="30"/>
@@ -29101,7 +29104,7 @@
       <c r="B47" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="C47" s="10" t="n">
+      <c r="C47" s="11" t="n">
         <v>46</v>
       </c>
       <c r="D47" s="30"/>
@@ -29114,7 +29117,7 @@
       <c r="B48" s="29" t="s">
         <v>303</v>
       </c>
-      <c r="C48" s="10" t="n">
+      <c r="C48" s="11" t="n">
         <v>47</v>
       </c>
       <c r="D48" s="30"/>
@@ -29127,7 +29130,7 @@
       <c r="B49" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="C49" s="10" t="n">
+      <c r="C49" s="11" t="n">
         <v>48</v>
       </c>
       <c r="D49" s="30"/>
@@ -29140,7 +29143,7 @@
       <c r="B50" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="C50" s="10" t="n">
+      <c r="C50" s="11" t="n">
         <v>49</v>
       </c>
       <c r="D50" s="30"/>
@@ -29153,7 +29156,7 @@
       <c r="B51" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="C51" s="10" t="n">
+      <c r="C51" s="11" t="n">
         <v>50</v>
       </c>
       <c r="D51" s="30"/>
@@ -29166,7 +29169,7 @@
       <c r="B52" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="C52" s="10" t="n">
+      <c r="C52" s="11" t="n">
         <v>51</v>
       </c>
       <c r="D52" s="21"/>
@@ -29179,7 +29182,7 @@
       <c r="B53" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="C53" s="10" t="n">
+      <c r="C53" s="11" t="n">
         <v>52</v>
       </c>
       <c r="D53" s="21"/>
@@ -29192,7 +29195,7 @@
       <c r="B54" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="C54" s="10" t="n">
+      <c r="C54" s="11" t="n">
         <v>53</v>
       </c>
       <c r="D54" s="21"/>
@@ -29205,7 +29208,7 @@
       <c r="B55" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C55" s="10" t="n">
+      <c r="C55" s="11" t="n">
         <v>54</v>
       </c>
     </row>
@@ -29216,7 +29219,7 @@
       <c r="B56" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="C56" s="10" t="n">
+      <c r="C56" s="11" t="n">
         <v>54</v>
       </c>
     </row>
@@ -29227,7 +29230,7 @@
       <c r="B57" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="C57" s="10" t="n">
+      <c r="C57" s="11" t="n">
         <v>55</v>
       </c>
     </row>
@@ -29238,7 +29241,7 @@
       <c r="B58" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="C58" s="10" t="n">
+      <c r="C58" s="11" t="n">
         <v>56</v>
       </c>
     </row>
@@ -29249,7 +29252,7 @@
       <c r="B59" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="C59" s="10" t="n">
+      <c r="C59" s="11" t="n">
         <v>57</v>
       </c>
     </row>
@@ -29260,7 +29263,7 @@
       <c r="B60" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="C60" s="10" t="n">
+      <c r="C60" s="11" t="n">
         <v>58</v>
       </c>
     </row>
@@ -29271,7 +29274,7 @@
       <c r="B61" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="C61" s="10" t="n">
+      <c r="C61" s="11" t="n">
         <v>59</v>
       </c>
     </row>
@@ -29282,7 +29285,7 @@
       <c r="B62" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="C62" s="10" t="n">
+      <c r="C62" s="11" t="n">
         <v>60</v>
       </c>
     </row>
@@ -29511,17 +29514,17 @@
   </sheetPr>
   <dimension ref="A1:AMH43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
@@ -30895,7 +30898,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D43"/>
+  <autoFilter ref="A1:D41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -30920,8 +30923,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="45.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.64372469635628"/>
@@ -31716,7 +31719,7 @@
       <c r="B72" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="C72" s="10" t="n">
+      <c r="C72" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31727,7 +31730,7 @@
       <c r="B73" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C73" s="10" t="n">
+      <c r="C73" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31738,7 +31741,7 @@
       <c r="B74" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C74" s="10" t="n">
+      <c r="C74" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31749,7 +31752,7 @@
       <c r="B75" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C75" s="10" t="n">
+      <c r="C75" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31760,7 +31763,7 @@
       <c r="B76" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C76" s="10" t="n">
+      <c r="C76" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31771,7 +31774,7 @@
       <c r="B77" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C77" s="10" t="n">
+      <c r="C77" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31782,7 +31785,7 @@
       <c r="B78" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C78" s="10" t="n">
+      <c r="C78" s="11" t="n">
         <v>30</v>
       </c>
     </row>
@@ -31793,7 +31796,7 @@
       <c r="B79" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C79" s="10" t="n">
+      <c r="C79" s="11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -31824,9 +31827,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.8785425101215"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -32465,17 +32468,17 @@
   </sheetPr>
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.0607287449393"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="94.9068825910931"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.5951417004049"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="95.7651821862348"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -32498,7 +32501,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>63</v>
@@ -32507,15 +32510,15 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>63</v>
@@ -32524,15 +32527,15 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>63</v>
@@ -32541,15 +32544,15 @@
         <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>377</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>110</v>
@@ -32558,15 +32561,15 @@
         <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>110</v>
@@ -32575,15 +32578,15 @@
         <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>381</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>110</v>
@@ -32592,15 +32595,15 @@
         <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>110</v>
@@ -32609,15 +32612,15 @@
         <v>46</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>385</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>110</v>
@@ -32626,15 +32629,15 @@
         <v>46</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>113</v>
@@ -32643,15 +32646,15 @@
         <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>113</v>
@@ -32660,15 +32663,15 @@
         <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>381</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>113</v>
@@ -32677,15 +32680,15 @@
         <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>113</v>
@@ -32694,15 +32697,15 @@
         <v>46</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>385</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>113</v>
@@ -32711,15 +32714,15 @@
         <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>15</v>
@@ -32728,15 +32731,15 @@
         <v>16</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>15</v>
@@ -32745,15 +32748,15 @@
         <v>16</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>15</v>
@@ -32762,15 +32765,15 @@
         <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>377</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>90</v>
@@ -32779,15 +32782,15 @@
         <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>90</v>
@@ -32796,15 +32799,15 @@
         <v>16</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>90</v>
@@ -32813,15 +32816,15 @@
         <v>46</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>377</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>122</v>
@@ -32830,15 +32833,15 @@
         <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>122</v>
@@ -32847,15 +32850,15 @@
         <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>389</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>122</v>
@@ -32864,15 +32867,15 @@
         <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>122</v>
@@ -32881,15 +32884,15 @@
         <v>46</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>122</v>
@@ -32898,15 +32901,15 @@
         <v>46</v>
       </c>
       <c r="D25" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>121</v>
@@ -32915,15 +32918,15 @@
         <v>16</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>121</v>
@@ -32932,15 +32935,15 @@
         <v>16</v>
       </c>
       <c r="D27" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>389</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>121</v>
@@ -32949,15 +32952,15 @@
         <v>46</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>121</v>
@@ -32966,15 +32969,15 @@
         <v>46</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>121</v>
@@ -32983,15 +32986,15 @@
         <v>46</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>55</v>
@@ -33000,15 +33003,15 @@
         <v>16</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>55</v>
@@ -33017,15 +33020,15 @@
         <v>16</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>55</v>
@@ -33034,15 +33037,15 @@
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>377</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>118</v>
@@ -33051,15 +33054,15 @@
         <v>16</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>118</v>
@@ -33068,15 +33071,15 @@
         <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>375</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>118</v>
@@ -33085,15 +33088,15 @@
         <v>46</v>
       </c>
       <c r="D36" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>377</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>126</v>
@@ -33102,15 +33105,15 @@
         <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>126</v>
@@ -33119,15 +33122,15 @@
         <v>16</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>389</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>126</v>
@@ -33136,15 +33139,15 @@
         <v>46</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>126</v>
@@ -33153,15 +33156,15 @@
         <v>46</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>126</v>
@@ -33170,15 +33173,15 @@
         <v>46</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>123</v>
@@ -33187,15 +33190,15 @@
         <v>16</v>
       </c>
       <c r="D42" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>123</v>
@@ -33204,15 +33207,15 @@
         <v>16</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>389</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>123</v>
@@ -33221,15 +33224,15 @@
         <v>46</v>
       </c>
       <c r="D44" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>123</v>
@@ -33238,15 +33241,15 @@
         <v>46</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>372</v>
+        <v>14</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>123</v>
@@ -33255,10 +33258,10 @@
         <v>46</v>
       </c>
       <c r="D46" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BATRU - P3 fixes
</commit_message>
<xml_diff>
--- a/Projects/BATRU/Data/P3_template.xlsx
+++ b/Projects/BATRU/Data/P3_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,6 +49,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sections!$A$1:$N$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
@@ -75,6 +76,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'SKU_Lists for sections'!$D$1:$H$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
@@ -101,6 +103,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Sequence list'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
@@ -127,6 +130,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'P3 SAS zone'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
@@ -153,6 +157,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Share priority'!$A$1:$C$1</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
@@ -179,6 +184,7 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Ean code'!$C$2:$D$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -190,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8940" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8940" uniqueCount="410">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -1290,9 +1296,6 @@
     <t xml:space="preserve">end_shelf</t>
   </si>
   <si>
-    <t xml:space="preserve">pos-000001</t>
-  </si>
-  <si>
     <t xml:space="preserve">product_english_name</t>
   </si>
   <si>
@@ -2013,22 +2016,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8947368421053"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3603238866397"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.9068825910931"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0161943319838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.9311740890688"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.0364372469636"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.0931174089069"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9068825910931"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.5465587044534"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.4048582995951"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47856,19 +47859,19 @@
   </sheetPr>
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F272" activeCellId="0" sqref="F272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2631578947368"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7125506072874"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54856,20 +54859,20 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9716599190283"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.91902834008097"/>
-    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1295546558704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4"/>
+    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56106,13 +56109,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.3967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8744939271255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58386,18 +58389,18 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2388663967611"/>
-    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.67206477732794"/>
-    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="55.1295546558704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="100" min="7" style="0" width="3.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1025" min="101" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59076,7 +59079,7 @@
         <v>233</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>366</v>
+        <v>234</v>
       </c>
       <c r="C62" s="24" t="n">
         <v>90</v>
@@ -59484,17 +59487,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.18218623481781"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8056680161943"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.9838056680162"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2" s="44" t="s">
         <v>163</v>
@@ -59502,7 +59505,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="45" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>278</v>
@@ -59550,10 +59553,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="45" t="s">
+        <v>368</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>369</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59585,7 +59588,7 @@
         <v>226</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59657,15 +59660,15 @@
         <v>169</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>373</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59742,10 +59745,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="45" t="s">
+        <v>374</v>
+      </c>
+      <c r="C33" s="45" t="s">
         <v>375</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59785,7 +59788,7 @@
         <v>353</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59818,7 +59821,7 @@
     </row>
     <row r="43" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C43" s="45"/>
     </row>
@@ -59828,10 +59831,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="45" t="s">
+        <v>378</v>
+      </c>
+      <c r="C45" s="45" t="s">
         <v>379</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -59887,7 +59890,7 @@
         <v>288</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60031,7 +60034,7 @@
         <v>323</v>
       </c>
       <c r="C70" s="45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60055,7 +60058,7 @@
         <v>326</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60071,7 +60074,7 @@
         <v>335</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60087,7 +60090,7 @@
         <v>336</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60103,7 +60106,7 @@
         <v>347</v>
       </c>
       <c r="C79" s="47" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -60132,12 +60135,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4817813765182"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.7692307692308"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.8987854251012"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="110.303643724696"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="115.400809716599"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60145,16 +60148,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>389</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60168,10 +60171,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60185,10 +60188,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60202,10 +60205,10 @@
         <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60219,10 +60222,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60236,10 +60239,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60253,10 +60256,10 @@
         <v>46</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60270,10 +60273,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60287,10 +60290,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60304,10 +60307,10 @@
         <v>46</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60321,10 +60324,10 @@
         <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>403</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60338,10 +60341,10 @@
         <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60355,10 +60358,10 @@
         <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60372,10 +60375,10 @@
         <v>16</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60389,10 +60392,10 @@
         <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60406,10 +60409,10 @@
         <v>46</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>403</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60423,10 +60426,10 @@
         <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60440,10 +60443,10 @@
         <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60457,10 +60460,10 @@
         <v>16</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60474,10 +60477,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60491,10 +60494,10 @@
         <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60508,10 +60511,10 @@
         <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60525,10 +60528,10 @@
         <v>46</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60542,10 +60545,10 @@
         <v>16</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60559,10 +60562,10 @@
         <v>16</v>
       </c>
       <c r="D25" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60576,10 +60579,10 @@
         <v>46</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60593,10 +60596,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60610,10 +60613,10 @@
         <v>46</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60627,10 +60630,10 @@
         <v>16</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60644,10 +60647,10 @@
         <v>16</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60661,10 +60664,10 @@
         <v>46</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60678,10 +60681,10 @@
         <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60695,10 +60698,10 @@
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60712,10 +60715,10 @@
         <v>16</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60729,10 +60732,10 @@
         <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60746,10 +60749,10 @@
         <v>46</v>
       </c>
       <c r="D36" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60763,10 +60766,10 @@
         <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60780,10 +60783,10 @@
         <v>16</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>393</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60797,10 +60800,10 @@
         <v>46</v>
       </c>
       <c r="D39" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>395</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60814,10 +60817,10 @@
         <v>16</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60831,10 +60834,10 @@
         <v>16</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60848,10 +60851,10 @@
         <v>46</v>
       </c>
       <c r="D42" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60865,10 +60868,10 @@
         <v>46</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60882,10 +60885,10 @@
         <v>46</v>
       </c>
       <c r="D44" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60899,10 +60902,10 @@
         <v>16</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60916,10 +60919,10 @@
         <v>16</v>
       </c>
       <c r="D46" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>407</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60933,10 +60936,10 @@
         <v>46</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60950,10 +60953,10 @@
         <v>46</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>409</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60967,10 +60970,10 @@
         <v>46</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>405</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>